<commit_message>
Add 100 magic items to Arcane Rating
</commit_message>
<xml_diff>
--- a/Arcane Artifacts Rating.xlsx
+++ b/Arcane Artifacts Rating.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtisdavid\Documents\personal\dnd-material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C94230-9491-478A-AA3E-68C062A40015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699AE2D7-A1E7-4BFC-98B5-CBA7150723CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F6E45A8-D54F-40B1-A986-0B1DDD400792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="33">
   <si>
     <t>Ring</t>
   </si>
@@ -95,7 +95,46 @@
     <t>Lip Ring</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Cloak</t>
+  </si>
+  <si>
+    <t>Hat</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Scarf</t>
+  </si>
+  <si>
+    <t>Cowl</t>
+  </si>
+  <si>
+    <t>Chaps</t>
+  </si>
+  <si>
+    <t>Apron</t>
+  </si>
+  <si>
+    <t>Goggles</t>
+  </si>
+  <si>
+    <t>Overalls</t>
+  </si>
+  <si>
+    <t>Mask</t>
   </si>
 </sst>
 </file>
@@ -447,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60572420-D8A5-49A0-95FE-F8B2A7A6A088}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="H186" sqref="H186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,6 +630,15 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1856,8 +1904,1404 @@
       <c r="A101" t="s">
         <v>19</v>
       </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>19</v>
+      </c>
+      <c r="B106">
+        <v>3</v>
+      </c>
+      <c r="C106" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>19</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>19</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>19</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>20</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>20</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>20</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>8</v>
+      </c>
+      <c r="D114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>20</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>20</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>20</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>20</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>20</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>20</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>21</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>21</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>21</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D123" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>21</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>8</v>
+      </c>
+      <c r="D124" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>21</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>21</v>
+      </c>
+      <c r="B126">
+        <v>2</v>
+      </c>
+      <c r="C126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>21</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>21</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>21</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>21</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>8</v>
+      </c>
+      <c r="D130" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>22</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>22</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132" t="s">
+        <v>8</v>
+      </c>
+      <c r="D132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>22</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>8</v>
+      </c>
+      <c r="D133" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>22</v>
+      </c>
+      <c r="B134">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
+        <v>8</v>
+      </c>
+      <c r="D134" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>22</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+      <c r="C135" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>22</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>8</v>
+      </c>
+      <c r="D136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>1</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>22</v>
+      </c>
+      <c r="B138">
+        <v>3</v>
+      </c>
+      <c r="C138" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>22</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
+        <v>8</v>
+      </c>
+      <c r="D139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>22</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>9</v>
+      </c>
+      <c r="D140" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>22</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>8</v>
+      </c>
+      <c r="D141" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>22</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>22</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>22</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>22</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>22</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>8</v>
+      </c>
+      <c r="D146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>22</v>
+      </c>
+      <c r="B147">
+        <v>2</v>
+      </c>
+      <c r="C147" t="s">
+        <v>8</v>
+      </c>
+      <c r="D147" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>22</v>
+      </c>
+      <c r="B148">
+        <v>2</v>
+      </c>
+      <c r="C148" t="s">
+        <v>8</v>
+      </c>
+      <c r="D148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>22</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149" t="s">
+        <v>8</v>
+      </c>
+      <c r="D149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>22</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="C150" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>23</v>
+      </c>
+      <c r="B152">
+        <v>3</v>
+      </c>
+      <c r="C152" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>23</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+      <c r="C153" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>23</v>
+      </c>
+      <c r="B154">
+        <v>2</v>
+      </c>
+      <c r="C154" t="s">
+        <v>10</v>
+      </c>
+      <c r="D154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>23</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>8</v>
+      </c>
+      <c r="D155" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>23</v>
+      </c>
+      <c r="B156">
+        <v>2</v>
+      </c>
+      <c r="C156" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>23</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>23</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="C158" t="s">
+        <v>8</v>
+      </c>
+      <c r="D158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="C159" t="s">
+        <v>8</v>
+      </c>
+      <c r="D159" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>23</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>8</v>
+      </c>
+      <c r="D160" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>23</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="C161" t="s">
+        <v>8</v>
+      </c>
+      <c r="D161" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>23</v>
+      </c>
+      <c r="B162">
+        <v>2</v>
+      </c>
+      <c r="C162" t="s">
+        <v>8</v>
+      </c>
+      <c r="D162" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>23</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163" t="s">
+        <v>10</v>
+      </c>
+      <c r="D163" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>23</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164" t="s">
+        <v>8</v>
+      </c>
+      <c r="D164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>23</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>10</v>
+      </c>
+      <c r="D165" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>23</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="C166" t="s">
+        <v>8</v>
+      </c>
+      <c r="D166" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>23</v>
+      </c>
+      <c r="B167">
+        <v>3</v>
+      </c>
+      <c r="C167" t="s">
+        <v>10</v>
+      </c>
+      <c r="D167" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>23</v>
+      </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>8</v>
+      </c>
+      <c r="D168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>23</v>
+      </c>
+      <c r="B169">
+        <v>1</v>
+      </c>
+      <c r="C169" t="s">
+        <v>10</v>
+      </c>
+      <c r="D169" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>23</v>
+      </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
+      <c r="C170" t="s">
+        <v>10</v>
+      </c>
+      <c r="D170" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>24</v>
+      </c>
+      <c r="B171">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s">
+        <v>10</v>
+      </c>
+      <c r="D171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>24</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="C172" t="s">
+        <v>8</v>
+      </c>
+      <c r="D172" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>24</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="C173" t="s">
+        <v>8</v>
+      </c>
+      <c r="D173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>24</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="C174" t="s">
+        <v>8</v>
+      </c>
+      <c r="D174" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>24</v>
+      </c>
+      <c r="B175">
+        <v>1</v>
+      </c>
+      <c r="C175" t="s">
+        <v>8</v>
+      </c>
+      <c r="D175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>24</v>
+      </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="C176" t="s">
+        <v>8</v>
+      </c>
+      <c r="D176" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>24</v>
+      </c>
+      <c r="B177">
+        <v>2</v>
+      </c>
+      <c r="C177" t="s">
+        <v>8</v>
+      </c>
+      <c r="D177" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>24</v>
+      </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
+      <c r="C178" t="s">
+        <v>8</v>
+      </c>
+      <c r="D178" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>24</v>
+      </c>
+      <c r="B179">
+        <v>1</v>
+      </c>
+      <c r="C179" t="s">
+        <v>8</v>
+      </c>
+      <c r="D179" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>24</v>
+      </c>
+      <c r="B180">
+        <v>2</v>
+      </c>
+      <c r="C180" t="s">
+        <v>8</v>
+      </c>
+      <c r="D180" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>25</v>
+      </c>
+      <c r="B181">
+        <v>1</v>
+      </c>
+      <c r="C181" t="s">
+        <v>8</v>
+      </c>
+      <c r="D181" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>25</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="C182" t="s">
+        <v>8</v>
+      </c>
+      <c r="D182" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>25</v>
+      </c>
+      <c r="B183">
+        <v>1</v>
+      </c>
+      <c r="C183" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>25</v>
+      </c>
+      <c r="B184">
+        <v>1</v>
+      </c>
+      <c r="C184" t="s">
+        <v>10</v>
+      </c>
+      <c r="D184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>25</v>
+      </c>
+      <c r="B185">
+        <v>2</v>
+      </c>
+      <c r="C185" t="s">
+        <v>10</v>
+      </c>
+      <c r="D185" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>25</v>
+      </c>
+      <c r="B186">
+        <v>1</v>
+      </c>
+      <c r="C186" t="s">
+        <v>8</v>
+      </c>
+      <c r="D186" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>25</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+      <c r="C187" t="s">
+        <v>8</v>
+      </c>
+      <c r="D187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>25</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188" t="s">
+        <v>8</v>
+      </c>
+      <c r="D188" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>25</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="C189" t="s">
+        <v>8</v>
+      </c>
+      <c r="D189" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>25</v>
+      </c>
+      <c r="B190">
+        <v>2</v>
+      </c>
+      <c r="C190" t="s">
+        <v>10</v>
+      </c>
+      <c r="D190" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>26</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="C191" t="s">
+        <v>10</v>
+      </c>
+      <c r="D191" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>27</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="C192" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>28</v>
+      </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="C193" t="s">
+        <v>8</v>
+      </c>
+      <c r="D193" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>29</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+      <c r="C194" t="s">
+        <v>8</v>
+      </c>
+      <c r="D194" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>30</v>
+      </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
+      <c r="C195" t="s">
+        <v>10</v>
+      </c>
+      <c r="D195" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>31</v>
+      </c>
+      <c r="B196">
+        <v>1</v>
+      </c>
+      <c r="C196" t="s">
+        <v>8</v>
+      </c>
+      <c r="D196" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>32</v>
+      </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
+      <c r="C197" t="s">
+        <v>8</v>
+      </c>
+      <c r="D197" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>32</v>
+      </c>
+      <c r="B198">
+        <v>1</v>
+      </c>
+      <c r="C198" t="s">
+        <v>8</v>
+      </c>
+      <c r="D198" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>32</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="C199" t="s">
+        <v>8</v>
+      </c>
+      <c r="D199" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>32</v>
+      </c>
+      <c r="B200">
+        <v>1</v>
+      </c>
+      <c r="C200" t="s">
+        <v>8</v>
+      </c>
+      <c r="D200" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 100 more items
</commit_message>
<xml_diff>
--- a/Arcane Artifacts Rating.xlsx
+++ b/Arcane Artifacts Rating.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clair\Documents\dnd-material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quazn\Documents\dnd-material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638D3259-A678-4EDD-A5D4-29F28E27FFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD96256-D106-4EB8-A90B-8950E73933AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F6E45A8-D54F-40B1-A986-0B1DDD400792}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9F6E45A8-D54F-40B1-A986-0B1DDD400792}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="45">
   <si>
     <t>Ring</t>
   </si>
@@ -527,19 +527,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60572420-D8A5-49A0-95FE-F8B2A7A6A088}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="H290" sqref="H290"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -556,7 +556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -590,7 +590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -607,7 +607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -641,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -658,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -675,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -692,7 +692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -709,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -743,7 +743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -760,7 +760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -777,7 +777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -794,7 +794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -811,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -828,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -862,7 +862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -879,7 +879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -896,7 +896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -913,7 +913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -930,7 +930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -947,7 +947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -964,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -981,7 +981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -998,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -4075,748 +4075,1585 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
       <c r="B209" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C209">
+        <v>2</v>
+      </c>
+      <c r="D209" t="s">
+        <v>10</v>
+      </c>
+      <c r="E209" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
       <c r="B210" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C210">
+        <v>3</v>
+      </c>
+      <c r="D210" t="s">
+        <v>8</v>
+      </c>
+      <c r="E210" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
       <c r="B211" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C211">
+        <v>1</v>
+      </c>
+      <c r="D211" t="s">
+        <v>8</v>
+      </c>
+      <c r="E211" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
       <c r="B212" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C212">
+        <v>1</v>
+      </c>
+      <c r="D212" t="s">
+        <v>10</v>
+      </c>
+      <c r="E212" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
       <c r="B213" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C213">
+        <v>2</v>
+      </c>
+      <c r="D213" t="s">
+        <v>8</v>
+      </c>
+      <c r="E213" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
       <c r="B214" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C214">
+        <v>2</v>
+      </c>
+      <c r="D214" t="s">
+        <v>10</v>
+      </c>
+      <c r="E214" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
       <c r="B215" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C215">
+        <v>1</v>
+      </c>
+      <c r="D215" t="s">
+        <v>8</v>
+      </c>
+      <c r="E215" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
       <c r="B216" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216" t="s">
+        <v>8</v>
+      </c>
+      <c r="E216" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
       <c r="B217" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C217">
+        <v>1</v>
+      </c>
+      <c r="D217" t="s">
+        <v>8</v>
+      </c>
+      <c r="E217" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
       <c r="B218" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C218">
+        <v>1</v>
+      </c>
+      <c r="D218" t="s">
+        <v>8</v>
+      </c>
+      <c r="E218" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
       <c r="B219" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C219">
+        <v>1</v>
+      </c>
+      <c r="D219" t="s">
+        <v>10</v>
+      </c>
+      <c r="E219" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
       <c r="B220" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C220">
+        <v>2</v>
+      </c>
+      <c r="D220" t="s">
+        <v>10</v>
+      </c>
+      <c r="E220" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
       <c r="B221" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C221">
+        <v>2</v>
+      </c>
+      <c r="D221" t="s">
+        <v>8</v>
+      </c>
+      <c r="E221" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
       <c r="B222" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C222">
+        <v>2</v>
+      </c>
+      <c r="D222" t="s">
+        <v>8</v>
+      </c>
+      <c r="E222" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
       <c r="B223" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C223">
+        <v>2</v>
+      </c>
+      <c r="D223" t="s">
+        <v>10</v>
+      </c>
+      <c r="E223" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
       <c r="B224" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C224">
+        <v>2</v>
+      </c>
+      <c r="D224" t="s">
+        <v>10</v>
+      </c>
+      <c r="E224" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
       <c r="B225" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225" t="s">
+        <v>10</v>
+      </c>
+      <c r="E225" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
       <c r="B226" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C226">
+        <v>1</v>
+      </c>
+      <c r="D226" t="s">
+        <v>10</v>
+      </c>
+      <c r="E226" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
       <c r="B227" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C227">
+        <v>2</v>
+      </c>
+      <c r="D227" t="s">
+        <v>10</v>
+      </c>
+      <c r="E227" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
       <c r="B228" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C228">
+        <v>1</v>
+      </c>
+      <c r="D228" t="s">
+        <v>10</v>
+      </c>
+      <c r="E228" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
       <c r="B229" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C229">
+        <v>2</v>
+      </c>
+      <c r="D229" t="s">
+        <v>10</v>
+      </c>
+      <c r="E229" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
       <c r="B230" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C230">
+        <v>1</v>
+      </c>
+      <c r="D230" t="s">
+        <v>10</v>
+      </c>
+      <c r="E230" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
       <c r="B231" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C231">
+        <v>1</v>
+      </c>
+      <c r="D231" t="s">
+        <v>10</v>
+      </c>
+      <c r="E231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
       <c r="B232" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C232">
+        <v>3</v>
+      </c>
+      <c r="D232" t="s">
+        <v>10</v>
+      </c>
+      <c r="E232" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
       <c r="B233" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C233">
+        <v>1</v>
+      </c>
+      <c r="D233" t="s">
+        <v>10</v>
+      </c>
+      <c r="E233" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
       <c r="B234" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C234">
+        <v>3</v>
+      </c>
+      <c r="D234" t="s">
+        <v>10</v>
+      </c>
+      <c r="E234" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
       <c r="B235" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C235">
+        <v>1</v>
+      </c>
+      <c r="D235" t="s">
+        <v>8</v>
+      </c>
+      <c r="E235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
       <c r="B236" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C236">
+        <v>1</v>
+      </c>
+      <c r="D236" t="s">
+        <v>10</v>
+      </c>
+      <c r="E236" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
       <c r="B237" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C237">
+        <v>2</v>
+      </c>
+      <c r="D237" t="s">
+        <v>10</v>
+      </c>
+      <c r="E237" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
       <c r="B238" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C238">
+        <v>2</v>
+      </c>
+      <c r="D238" t="s">
+        <v>10</v>
+      </c>
+      <c r="E238" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
       <c r="B239" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C239">
+        <v>2</v>
+      </c>
+      <c r="D239" t="s">
+        <v>8</v>
+      </c>
+      <c r="E239" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
       <c r="B240" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240" t="s">
+        <v>8</v>
+      </c>
+      <c r="E240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
       <c r="B241" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C241">
+        <v>2</v>
+      </c>
+      <c r="D241" t="s">
+        <v>10</v>
+      </c>
+      <c r="E241" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
       <c r="B242" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="D242" t="s">
+        <v>8</v>
+      </c>
+      <c r="E242" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
       <c r="B243" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C243">
+        <v>1</v>
+      </c>
+      <c r="D243" t="s">
+        <v>10</v>
+      </c>
+      <c r="E243" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
       <c r="B244" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C244">
+        <v>1</v>
+      </c>
+      <c r="D244" t="s">
+        <v>10</v>
+      </c>
+      <c r="E244" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
       <c r="B245" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245" t="s">
+        <v>8</v>
+      </c>
+      <c r="E245" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
       <c r="B246" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C246">
+        <v>4</v>
+      </c>
+      <c r="D246" t="s">
+        <v>9</v>
+      </c>
+      <c r="E246" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
       <c r="B247" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C247">
+        <v>3</v>
+      </c>
+      <c r="D247" t="s">
+        <v>10</v>
+      </c>
+      <c r="E247" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
       <c r="B248" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248" t="s">
+        <v>8</v>
+      </c>
+      <c r="E248" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
       <c r="B249" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
       <c r="B250" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C250">
+        <v>2</v>
+      </c>
+      <c r="D250" t="s">
+        <v>9</v>
+      </c>
+      <c r="E250" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
       <c r="B251" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251" t="s">
+        <v>8</v>
+      </c>
+      <c r="E251" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
       <c r="B252" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C252">
+        <v>1</v>
+      </c>
+      <c r="D252" t="s">
+        <v>8</v>
+      </c>
+      <c r="E252" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
       <c r="B253" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C253">
+        <v>1</v>
+      </c>
+      <c r="D253" t="s">
+        <v>8</v>
+      </c>
+      <c r="E253" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
       <c r="B254" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C254">
+        <v>2</v>
+      </c>
+      <c r="D254" t="s">
+        <v>9</v>
+      </c>
+      <c r="E254" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
       <c r="B255" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C255">
+        <v>2</v>
+      </c>
+      <c r="D255" t="s">
+        <v>10</v>
+      </c>
+      <c r="E255" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
       <c r="B256" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C256">
+        <v>3</v>
+      </c>
+      <c r="D256" t="s">
+        <v>10</v>
+      </c>
+      <c r="E256" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>256</v>
       </c>
       <c r="B257" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C257">
+        <v>1</v>
+      </c>
+      <c r="D257" t="s">
+        <v>8</v>
+      </c>
+      <c r="E257" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>257</v>
       </c>
       <c r="B258" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C258">
+        <v>2</v>
+      </c>
+      <c r="D258" t="s">
+        <v>10</v>
+      </c>
+      <c r="E258" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>258</v>
       </c>
       <c r="B259" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C259">
+        <v>2</v>
+      </c>
+      <c r="D259" t="s">
+        <v>8</v>
+      </c>
+      <c r="E259" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>259</v>
       </c>
       <c r="B260" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C260">
+        <v>1</v>
+      </c>
+      <c r="D260" t="s">
+        <v>10</v>
+      </c>
+      <c r="E260" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>260</v>
       </c>
       <c r="B261" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C261">
+        <v>1</v>
+      </c>
+      <c r="D261" t="s">
+        <v>8</v>
+      </c>
+      <c r="E261" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>261</v>
       </c>
       <c r="B262" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C262">
+        <v>3</v>
+      </c>
+      <c r="D262" t="s">
+        <v>8</v>
+      </c>
+      <c r="E262" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>262</v>
       </c>
       <c r="B263" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C263">
+        <v>1</v>
+      </c>
+      <c r="D263" t="s">
+        <v>8</v>
+      </c>
+      <c r="E263" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>263</v>
       </c>
       <c r="B264" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C264">
+        <v>1</v>
+      </c>
+      <c r="D264" t="s">
+        <v>10</v>
+      </c>
+      <c r="E264" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>264</v>
       </c>
       <c r="B265" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C265">
+        <v>2</v>
+      </c>
+      <c r="D265" t="s">
+        <v>10</v>
+      </c>
+      <c r="E265" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>265</v>
       </c>
       <c r="B266" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C266">
+        <v>1</v>
+      </c>
+      <c r="D266" t="s">
+        <v>8</v>
+      </c>
+      <c r="E266" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>266</v>
       </c>
       <c r="B267" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C267">
+        <v>1</v>
+      </c>
+      <c r="D267" t="s">
+        <v>10</v>
+      </c>
+      <c r="E267" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>267</v>
       </c>
       <c r="B268" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C268">
+        <v>2</v>
+      </c>
+      <c r="D268" t="s">
+        <v>10</v>
+      </c>
+      <c r="E268" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>268</v>
       </c>
       <c r="B269" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C269">
+        <v>1</v>
+      </c>
+      <c r="D269" t="s">
+        <v>10</v>
+      </c>
+      <c r="E269" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>269</v>
       </c>
       <c r="B270" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C270">
+        <v>3</v>
+      </c>
+      <c r="D270" t="s">
+        <v>10</v>
+      </c>
+      <c r="E270" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>270</v>
       </c>
       <c r="B271" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C271">
+        <v>1</v>
+      </c>
+      <c r="D271" t="s">
+        <v>10</v>
+      </c>
+      <c r="E271" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>271</v>
       </c>
       <c r="B272" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C272">
+        <v>1</v>
+      </c>
+      <c r="D272" t="s">
+        <v>10</v>
+      </c>
+      <c r="E272" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>272</v>
       </c>
       <c r="B273" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C273">
+        <v>2</v>
+      </c>
+      <c r="D273" t="s">
+        <v>8</v>
+      </c>
+      <c r="E273" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>273</v>
       </c>
       <c r="B274" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C274">
+        <v>3</v>
+      </c>
+      <c r="D274" t="s">
+        <v>10</v>
+      </c>
+      <c r="E274" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>274</v>
       </c>
       <c r="B275" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C275">
+        <v>1</v>
+      </c>
+      <c r="D275" t="s">
+        <v>8</v>
+      </c>
+      <c r="E275" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>275</v>
       </c>
       <c r="B276" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C276">
+        <v>1</v>
+      </c>
+      <c r="D276" t="s">
+        <v>8</v>
+      </c>
+      <c r="E276" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>276</v>
       </c>
       <c r="B277" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C277">
+        <v>1</v>
+      </c>
+      <c r="D277" t="s">
+        <v>10</v>
+      </c>
+      <c r="E277" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
       <c r="B278" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1</v>
+      </c>
+      <c r="D278" t="s">
+        <v>1</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
       <c r="B279" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C279">
+        <v>1</v>
+      </c>
+      <c r="D279" t="s">
+        <v>10</v>
+      </c>
+      <c r="E279" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>279</v>
       </c>
       <c r="B280" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C280">
+        <v>1</v>
+      </c>
+      <c r="D280" t="s">
+        <v>10</v>
+      </c>
+      <c r="E280" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>280</v>
       </c>
       <c r="B281" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C281">
+        <v>2</v>
+      </c>
+      <c r="D281" t="s">
+        <v>10</v>
+      </c>
+      <c r="E281" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>281</v>
       </c>
       <c r="B282" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C282">
+        <v>1</v>
+      </c>
+      <c r="D282" t="s">
+        <v>8</v>
+      </c>
+      <c r="E282" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>282</v>
       </c>
       <c r="B283" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C283">
+        <v>1</v>
+      </c>
+      <c r="D283" t="s">
+        <v>8</v>
+      </c>
+      <c r="E283" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>283</v>
       </c>
       <c r="B284" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C284">
+        <v>2</v>
+      </c>
+      <c r="D284" t="s">
+        <v>9</v>
+      </c>
+      <c r="E284" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>284</v>
       </c>
       <c r="B285" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C285">
+        <v>2</v>
+      </c>
+      <c r="D285" t="s">
+        <v>10</v>
+      </c>
+      <c r="E285" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>285</v>
       </c>
       <c r="B286" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C286">
+        <v>1</v>
+      </c>
+      <c r="D286" t="s">
+        <v>10</v>
+      </c>
+      <c r="E286" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>286</v>
       </c>
       <c r="B287" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C287">
+        <v>1</v>
+      </c>
+      <c r="D287" t="s">
+        <v>8</v>
+      </c>
+      <c r="E287" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>287</v>
       </c>
       <c r="B288" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C288">
+        <v>1</v>
+      </c>
+      <c r="D288" t="s">
+        <v>8</v>
+      </c>
+      <c r="E288" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>288</v>
       </c>
       <c r="B289" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C289">
+        <v>1</v>
+      </c>
+      <c r="D289" t="s">
+        <v>8</v>
+      </c>
+      <c r="E289" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>289</v>
       </c>
       <c r="B290" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C290">
+        <v>2</v>
+      </c>
+      <c r="D290" t="s">
+        <v>8</v>
+      </c>
+      <c r="E290" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>290</v>
       </c>
       <c r="B291" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C291">
+        <v>1</v>
+      </c>
+      <c r="D291" t="s">
+        <v>8</v>
+      </c>
+      <c r="E291" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>291</v>
       </c>
       <c r="B292" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C292">
+        <v>1</v>
+      </c>
+      <c r="D292" t="s">
+        <v>10</v>
+      </c>
+      <c r="E292" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>292</v>
       </c>
       <c r="B293" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C293">
+        <v>2</v>
+      </c>
+      <c r="D293" t="s">
+        <v>10</v>
+      </c>
+      <c r="E293" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>293</v>
       </c>
       <c r="B294" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C294">
+        <v>3</v>
+      </c>
+      <c r="D294" t="s">
+        <v>10</v>
+      </c>
+      <c r="E294" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>294</v>
       </c>
       <c r="B295" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C295">
+        <v>2</v>
+      </c>
+      <c r="D295" t="s">
+        <v>10</v>
+      </c>
+      <c r="E295" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>295</v>
       </c>
       <c r="B296" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C296">
+        <v>1</v>
+      </c>
+      <c r="D296" t="s">
+        <v>8</v>
+      </c>
+      <c r="E296" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>296</v>
       </c>
       <c r="B297" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C297">
+        <v>1</v>
+      </c>
+      <c r="D297" t="s">
+        <v>10</v>
+      </c>
+      <c r="E297" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>297</v>
       </c>
       <c r="B298" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C298">
+        <v>1</v>
+      </c>
+      <c r="D298" t="s">
+        <v>8</v>
+      </c>
+      <c r="E298" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>298</v>
       </c>
       <c r="B299" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C299">
+        <v>2</v>
+      </c>
+      <c r="D299" t="s">
+        <v>10</v>
+      </c>
+      <c r="E299" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>299</v>
       </c>
       <c r="B300" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C300">
+        <v>1</v>
+      </c>
+      <c r="D300" t="s">
+        <v>10</v>
+      </c>
+      <c r="E300" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>300</v>
       </c>
       <c r="B301" t="s">
         <v>39</v>
+      </c>
+      <c r="C301">
+        <v>2</v>
+      </c>
+      <c r="D301" t="s">
+        <v>10</v>
+      </c>
+      <c r="E301" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add even more items
</commit_message>
<xml_diff>
--- a/Arcane Artifacts Rating.xlsx
+++ b/Arcane Artifacts Rating.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quazn\Documents\dnd-material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clair\Documents\dnd-material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD96256-D106-4EB8-A90B-8950E73933AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73A131-1421-49B9-929D-6D2E7B338EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9F6E45A8-D54F-40B1-A986-0B1DDD400792}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F6E45A8-D54F-40B1-A986-0B1DDD400792}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="68">
   <si>
     <t>Ring</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Greaves</t>
   </si>
   <si>
-    <t>Shields</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -174,6 +171,78 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+  <si>
+    <t>Knife</t>
+  </si>
+  <si>
+    <t>Sword</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Club</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Morning Start</t>
+  </si>
+  <si>
+    <t>Blackjack</t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Shillelagh</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Stave</t>
+  </si>
+  <si>
+    <t>Spear</t>
+  </si>
+  <si>
+    <t>Projectile</t>
+  </si>
+  <si>
+    <t>Chain</t>
+  </si>
+  <si>
+    <t>Whip</t>
+  </si>
+  <si>
+    <t>Sling</t>
+  </si>
+  <si>
+    <t>Garrote</t>
+  </si>
+  <si>
+    <t>Sickle</t>
+  </si>
+  <si>
+    <t>Trident</t>
+  </si>
+  <si>
+    <t>Blowgun</t>
+  </si>
+  <si>
+    <t>Net</t>
+  </si>
+  <si>
+    <t>Slingshot</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -525,38 +594,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60572420-D8A5-49A0-95FE-F8B2A7A6A088}">
-  <dimension ref="A1:E301"/>
+  <dimension ref="A1:G401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="H290" sqref="H290"/>
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="H367" sqref="H367"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -573,7 +642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -590,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -607,7 +676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -624,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -641,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -658,7 +727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -675,7 +744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -692,7 +761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -709,7 +778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -726,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -743,7 +812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -760,7 +829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -777,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -794,7 +863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -811,7 +880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -828,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -845,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -862,7 +931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -879,7 +948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -896,7 +965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -913,7 +982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -930,7 +999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -947,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -964,7 +1033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -981,7 +1050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -998,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1015,7 +1084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1032,7 +1101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1049,7 +1118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1066,7 +1135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1083,7 +1152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1100,7 +1169,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1117,7 +1186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1134,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1151,7 +1220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1168,7 +1237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1185,7 +1254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1202,7 +1271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1219,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1236,7 +1305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1253,7 +1322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1270,7 +1339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1287,7 +1356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1304,7 +1373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1321,7 +1390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1338,7 +1407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1355,7 +1424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1372,7 +1441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1389,7 +1458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1406,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1423,7 +1492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1440,7 +1509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1457,7 +1526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1474,7 +1543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1491,7 +1560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1508,7 +1577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1525,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1542,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1559,7 +1628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1576,7 +1645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1593,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1610,7 +1679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1627,7 +1696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1644,7 +1713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1661,7 +1730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1678,7 +1747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1695,7 +1764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1712,7 +1781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1729,7 +1798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1746,7 +1815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1763,7 +1832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1780,7 +1849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1797,7 +1866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1814,7 +1883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1831,7 +1900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1848,7 +1917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1865,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1882,7 +1951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1899,7 +1968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1916,7 +1985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1933,7 +2002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1950,7 +2019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1967,7 +2036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1984,7 +2053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2001,7 +2070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2018,7 +2087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2035,7 +2104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2052,7 +2121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2069,7 +2138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2086,7 +2155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2103,7 +2172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2120,7 +2189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2137,7 +2206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2154,7 +2223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2171,7 +2240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2188,7 +2257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2205,7 +2274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2222,7 +2291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2239,7 +2308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2256,7 +2325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2273,7 +2342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2290,7 +2359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2307,7 +2376,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2324,7 +2393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2341,7 +2410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2358,7 +2427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2375,7 +2444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2392,7 +2461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2409,7 +2478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2426,7 +2495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2443,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2460,7 +2529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2477,7 +2546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2494,7 +2563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2511,7 +2580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2528,7 +2597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2545,7 +2614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2562,7 +2631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2579,7 +2648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2596,7 +2665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2613,7 +2682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2630,7 +2699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2647,7 +2716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2664,7 +2733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2681,7 +2750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2698,7 +2767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2715,7 +2784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2732,7 +2801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -2749,7 +2818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2766,7 +2835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2783,7 +2852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2800,7 +2869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2817,7 +2886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2834,7 +2903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2851,7 +2920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2868,7 +2937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2885,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2902,7 +2971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -2919,7 +2988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -2936,7 +3005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -2953,7 +3022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -2970,7 +3039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -2987,7 +3056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3004,7 +3073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3021,7 +3090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3038,7 +3107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3055,7 +3124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3072,7 +3141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -3089,7 +3158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -3106,7 +3175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -3123,7 +3192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -3140,7 +3209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -3157,7 +3226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -3174,7 +3243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -3191,7 +3260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -3208,7 +3277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -3225,7 +3294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3242,7 +3311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3259,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3276,7 +3345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3293,7 +3362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3310,7 +3379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3327,7 +3396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3344,7 +3413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3361,7 +3430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3378,7 +3447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3395,7 +3464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3412,7 +3481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3429,7 +3498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3446,7 +3515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3463,7 +3532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3480,7 +3549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3497,7 +3566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3514,7 +3583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3531,7 +3600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3548,7 +3617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3565,7 +3634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3582,7 +3651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -3599,7 +3668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -3616,7 +3685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -3633,7 +3702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -3650,7 +3719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -3667,7 +3736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -3684,7 +3753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -3701,7 +3770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -3718,7 +3787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -3735,7 +3804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -3752,7 +3821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -3769,7 +3838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -3786,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -3803,7 +3872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
@@ -3820,7 +3889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
@@ -3837,7 +3906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
@@ -3854,7 +3923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
@@ -3871,7 +3940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
@@ -3888,7 +3957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
@@ -3905,7 +3974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
@@ -3922,7 +3991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
@@ -3939,7 +4008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
@@ -3956,7 +4025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
@@ -3973,7 +4042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
@@ -3990,7 +4059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
@@ -4007,7 +4076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
@@ -4024,7 +4093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
@@ -4041,7 +4110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
@@ -4058,7 +4127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>
@@ -4075,7 +4144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -4092,7 +4161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -4109,7 +4178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -4126,7 +4195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -4143,7 +4212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -4160,7 +4229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -4177,7 +4246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -4194,7 +4263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -4211,7 +4280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -4228,7 +4297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -4245,7 +4314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -4262,7 +4331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -4279,7 +4348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -4296,7 +4365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -4313,7 +4382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -4330,7 +4399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -4347,7 +4416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>224</v>
       </c>
@@ -4364,7 +4433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>225</v>
       </c>
@@ -4381,7 +4450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>226</v>
       </c>
@@ -4398,7 +4467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>227</v>
       </c>
@@ -4415,7 +4484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>228</v>
       </c>
@@ -4432,7 +4501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>229</v>
       </c>
@@ -4449,7 +4518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>230</v>
       </c>
@@ -4466,7 +4535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>231</v>
       </c>
@@ -4483,7 +4552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>232</v>
       </c>
@@ -4500,7 +4569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>233</v>
       </c>
@@ -4517,7 +4586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>234</v>
       </c>
@@ -4534,7 +4603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>235</v>
       </c>
@@ -4551,7 +4620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>236</v>
       </c>
@@ -4568,7 +4637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>237</v>
       </c>
@@ -4585,7 +4654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>238</v>
       </c>
@@ -4602,7 +4671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>239</v>
       </c>
@@ -4619,7 +4688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
@@ -4636,7 +4705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>241</v>
       </c>
@@ -4653,7 +4722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242</v>
       </c>
@@ -4670,7 +4739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>243</v>
       </c>
@@ -4687,7 +4756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>244</v>
       </c>
@@ -4704,7 +4773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>245</v>
       </c>
@@ -4721,7 +4790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>246</v>
       </c>
@@ -4738,7 +4807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>247</v>
       </c>
@@ -4755,7 +4824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>248</v>
       </c>
@@ -4772,7 +4841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>249</v>
       </c>
@@ -4789,7 +4858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>250</v>
       </c>
@@ -4806,7 +4875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>251</v>
       </c>
@@ -4823,7 +4892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252</v>
       </c>
@@ -4840,7 +4909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253</v>
       </c>
@@ -4857,7 +4926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>254</v>
       </c>
@@ -4874,7 +4943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>255</v>
       </c>
@@ -4891,7 +4960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>256</v>
       </c>
@@ -4908,7 +4977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>257</v>
       </c>
@@ -4925,7 +4994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>258</v>
       </c>
@@ -4942,7 +5011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>259</v>
       </c>
@@ -4959,7 +5028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>260</v>
       </c>
@@ -4976,7 +5045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>261</v>
       </c>
@@ -4993,7 +5062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>262</v>
       </c>
@@ -5010,7 +5079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>263</v>
       </c>
@@ -5027,7 +5096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>264</v>
       </c>
@@ -5044,7 +5113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>265</v>
       </c>
@@ -5061,7 +5130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>266</v>
       </c>
@@ -5078,7 +5147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>267</v>
       </c>
@@ -5095,7 +5164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>268</v>
       </c>
@@ -5112,7 +5181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>269</v>
       </c>
@@ -5129,7 +5198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>270</v>
       </c>
@@ -5146,7 +5215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>271</v>
       </c>
@@ -5163,7 +5232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>272</v>
       </c>
@@ -5180,7 +5249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>273</v>
       </c>
@@ -5197,7 +5266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>274</v>
       </c>
@@ -5214,7 +5283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>275</v>
       </c>
@@ -5231,7 +5300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>276</v>
       </c>
@@ -5248,7 +5317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>277</v>
       </c>
@@ -5265,7 +5334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>278</v>
       </c>
@@ -5282,7 +5351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>279</v>
       </c>
@@ -5299,7 +5368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>280</v>
       </c>
@@ -5316,7 +5385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>281</v>
       </c>
@@ -5333,7 +5402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>282</v>
       </c>
@@ -5350,7 +5419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>283</v>
       </c>
@@ -5367,7 +5436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>284</v>
       </c>
@@ -5384,7 +5453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>285</v>
       </c>
@@ -5401,7 +5470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>286</v>
       </c>
@@ -5418,7 +5487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>287</v>
       </c>
@@ -5435,7 +5504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>288</v>
       </c>
@@ -5452,7 +5521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>289</v>
       </c>
@@ -5469,7 +5538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>290</v>
       </c>
@@ -5486,12 +5555,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>291</v>
       </c>
       <c r="B292" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C292">
         <v>1</v>
@@ -5503,12 +5572,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>292</v>
       </c>
       <c r="B293" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C293">
         <v>2</v>
@@ -5520,12 +5589,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>293</v>
       </c>
       <c r="B294" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C294">
         <v>3</v>
@@ -5537,12 +5606,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>294</v>
       </c>
       <c r="B295" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C295">
         <v>2</v>
@@ -5554,12 +5623,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>295</v>
       </c>
       <c r="B296" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C296">
         <v>1</v>
@@ -5571,12 +5640,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C297">
         <v>1</v>
@@ -5588,12 +5657,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>297</v>
       </c>
       <c r="B298" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C298">
         <v>1</v>
@@ -5602,15 +5671,15 @@
         <v>8</v>
       </c>
       <c r="E298" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>298</v>
       </c>
       <c r="B299" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C299">
         <v>2</v>
@@ -5622,12 +5691,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>299</v>
       </c>
       <c r="B300" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C300">
         <v>1</v>
@@ -5639,12 +5708,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>300</v>
       </c>
       <c r="B301" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C301">
         <v>2</v>
@@ -5654,6 +5723,1352 @@
       </c>
       <c r="E301" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>301</v>
+      </c>
+      <c r="B302" t="s">
+        <v>46</v>
+      </c>
+      <c r="C302">
+        <v>4</v>
+      </c>
+      <c r="D302" t="s">
+        <v>10</v>
+      </c>
+      <c r="E302" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>302</v>
+      </c>
+      <c r="B303" t="s">
+        <v>46</v>
+      </c>
+      <c r="C303">
+        <v>1</v>
+      </c>
+      <c r="D303" t="s">
+        <v>10</v>
+      </c>
+      <c r="E303" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>303</v>
+      </c>
+      <c r="B304" t="s">
+        <v>46</v>
+      </c>
+      <c r="C304">
+        <v>2</v>
+      </c>
+      <c r="D304" t="s">
+        <v>10</v>
+      </c>
+      <c r="E304" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>304</v>
+      </c>
+      <c r="B305" t="s">
+        <v>46</v>
+      </c>
+      <c r="C305">
+        <v>1</v>
+      </c>
+      <c r="D305" t="s">
+        <v>10</v>
+      </c>
+      <c r="E305" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>305</v>
+      </c>
+      <c r="B306" t="s">
+        <v>46</v>
+      </c>
+      <c r="C306">
+        <v>2</v>
+      </c>
+      <c r="D306" t="s">
+        <v>10</v>
+      </c>
+      <c r="E306" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A307">
+        <v>306</v>
+      </c>
+      <c r="B307" t="s">
+        <v>46</v>
+      </c>
+      <c r="C307">
+        <v>2</v>
+      </c>
+      <c r="D307" t="s">
+        <v>10</v>
+      </c>
+      <c r="E307" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>307</v>
+      </c>
+      <c r="B308" t="s">
+        <v>46</v>
+      </c>
+      <c r="C308">
+        <v>1</v>
+      </c>
+      <c r="D308" t="s">
+        <v>10</v>
+      </c>
+      <c r="E308" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A309">
+        <v>308</v>
+      </c>
+      <c r="B309" t="s">
+        <v>46</v>
+      </c>
+      <c r="C309">
+        <v>3</v>
+      </c>
+      <c r="D309" t="s">
+        <v>10</v>
+      </c>
+      <c r="E309" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A310">
+        <v>309</v>
+      </c>
+      <c r="B310" t="s">
+        <v>46</v>
+      </c>
+      <c r="C310">
+        <v>1</v>
+      </c>
+      <c r="D310" t="s">
+        <v>8</v>
+      </c>
+      <c r="E310" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A311">
+        <v>310</v>
+      </c>
+      <c r="B311" t="s">
+        <v>46</v>
+      </c>
+      <c r="C311">
+        <v>2</v>
+      </c>
+      <c r="D311" t="s">
+        <v>10</v>
+      </c>
+      <c r="E311" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A312">
+        <v>311</v>
+      </c>
+      <c r="B312" t="s">
+        <v>46</v>
+      </c>
+      <c r="C312">
+        <v>3</v>
+      </c>
+      <c r="D312" t="s">
+        <v>10</v>
+      </c>
+      <c r="E312" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A313">
+        <v>312</v>
+      </c>
+      <c r="B313" t="s">
+        <v>46</v>
+      </c>
+      <c r="C313">
+        <v>2</v>
+      </c>
+      <c r="D313" t="s">
+        <v>10</v>
+      </c>
+      <c r="E313" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A314">
+        <v>313</v>
+      </c>
+      <c r="B314" t="s">
+        <v>46</v>
+      </c>
+      <c r="C314">
+        <v>1</v>
+      </c>
+      <c r="D314" t="s">
+        <v>10</v>
+      </c>
+      <c r="E314" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A315">
+        <v>314</v>
+      </c>
+      <c r="B315" t="s">
+        <v>46</v>
+      </c>
+      <c r="C315">
+        <v>3</v>
+      </c>
+      <c r="D315" t="s">
+        <v>9</v>
+      </c>
+      <c r="E315" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A316">
+        <v>315</v>
+      </c>
+      <c r="B316" t="s">
+        <v>46</v>
+      </c>
+      <c r="C316">
+        <v>1</v>
+      </c>
+      <c r="D316" t="s">
+        <v>8</v>
+      </c>
+      <c r="E316" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A317">
+        <v>316</v>
+      </c>
+      <c r="B317" t="s">
+        <v>46</v>
+      </c>
+      <c r="C317">
+        <v>1</v>
+      </c>
+      <c r="D317" t="s">
+        <v>10</v>
+      </c>
+      <c r="E317" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A318">
+        <v>317</v>
+      </c>
+      <c r="B318" t="s">
+        <v>46</v>
+      </c>
+      <c r="C318">
+        <v>1</v>
+      </c>
+      <c r="D318" t="s">
+        <v>10</v>
+      </c>
+      <c r="E318" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A319">
+        <v>318</v>
+      </c>
+      <c r="B319" t="s">
+        <v>1</v>
+      </c>
+      <c r="C319" t="s">
+        <v>1</v>
+      </c>
+      <c r="D319" t="s">
+        <v>1</v>
+      </c>
+      <c r="E319" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A320">
+        <v>319</v>
+      </c>
+      <c r="B320" t="s">
+        <v>46</v>
+      </c>
+      <c r="C320">
+        <v>2</v>
+      </c>
+      <c r="D320" t="s">
+        <v>10</v>
+      </c>
+      <c r="E320" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A321">
+        <v>320</v>
+      </c>
+      <c r="B321" t="s">
+        <v>46</v>
+      </c>
+      <c r="C321">
+        <v>2</v>
+      </c>
+      <c r="D321" t="s">
+        <v>10</v>
+      </c>
+      <c r="E321" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A322">
+        <v>321</v>
+      </c>
+      <c r="B322" t="s">
+        <v>45</v>
+      </c>
+      <c r="C322">
+        <v>2</v>
+      </c>
+      <c r="D322" t="s">
+        <v>10</v>
+      </c>
+      <c r="E322" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A323">
+        <v>322</v>
+      </c>
+      <c r="B323" t="s">
+        <v>45</v>
+      </c>
+      <c r="C323">
+        <v>2</v>
+      </c>
+      <c r="D323" t="s">
+        <v>10</v>
+      </c>
+      <c r="E323" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A324">
+        <v>323</v>
+      </c>
+      <c r="B324" t="s">
+        <v>45</v>
+      </c>
+      <c r="C324">
+        <v>1</v>
+      </c>
+      <c r="D324" t="s">
+        <v>10</v>
+      </c>
+      <c r="E324" t="s">
+        <v>3</v>
+      </c>
+      <c r="G324" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A325">
+        <v>324</v>
+      </c>
+      <c r="B325" t="s">
+        <v>45</v>
+      </c>
+      <c r="C325">
+        <v>1</v>
+      </c>
+      <c r="D325" t="s">
+        <v>8</v>
+      </c>
+      <c r="E325" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A326">
+        <v>325</v>
+      </c>
+      <c r="B326" t="s">
+        <v>45</v>
+      </c>
+      <c r="C326">
+        <v>2</v>
+      </c>
+      <c r="D326" t="s">
+        <v>8</v>
+      </c>
+      <c r="E326" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A327">
+        <v>326</v>
+      </c>
+      <c r="B327" t="s">
+        <v>45</v>
+      </c>
+      <c r="C327">
+        <v>1</v>
+      </c>
+      <c r="D327" t="s">
+        <v>8</v>
+      </c>
+      <c r="E327" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A328">
+        <v>327</v>
+      </c>
+      <c r="B328" t="s">
+        <v>45</v>
+      </c>
+      <c r="C328">
+        <v>1</v>
+      </c>
+      <c r="D328" t="s">
+        <v>8</v>
+      </c>
+      <c r="E328" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A329">
+        <v>328</v>
+      </c>
+      <c r="B329" t="s">
+        <v>45</v>
+      </c>
+      <c r="C329">
+        <v>1</v>
+      </c>
+      <c r="D329" t="s">
+        <v>8</v>
+      </c>
+      <c r="E329" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A330">
+        <v>329</v>
+      </c>
+      <c r="B330" t="s">
+        <v>45</v>
+      </c>
+      <c r="C330">
+        <v>2</v>
+      </c>
+      <c r="D330" t="s">
+        <v>8</v>
+      </c>
+      <c r="E330" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A331">
+        <v>330</v>
+      </c>
+      <c r="B331" t="s">
+        <v>45</v>
+      </c>
+      <c r="C331">
+        <v>1</v>
+      </c>
+      <c r="D331" t="s">
+        <v>8</v>
+      </c>
+      <c r="E331" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A332">
+        <v>331</v>
+      </c>
+      <c r="B332" t="s">
+        <v>44</v>
+      </c>
+      <c r="C332">
+        <v>1</v>
+      </c>
+      <c r="D332" t="s">
+        <v>8</v>
+      </c>
+      <c r="E332" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A333">
+        <v>332</v>
+      </c>
+      <c r="B333" t="s">
+        <v>44</v>
+      </c>
+      <c r="C333">
+        <v>1</v>
+      </c>
+      <c r="D333" t="s">
+        <v>10</v>
+      </c>
+      <c r="E333" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>333</v>
+      </c>
+      <c r="B334" t="s">
+        <v>44</v>
+      </c>
+      <c r="C334">
+        <v>1</v>
+      </c>
+      <c r="D334" t="s">
+        <v>10</v>
+      </c>
+      <c r="E334" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>334</v>
+      </c>
+      <c r="B335" t="s">
+        <v>44</v>
+      </c>
+      <c r="C335">
+        <v>3</v>
+      </c>
+      <c r="D335" t="s">
+        <v>10</v>
+      </c>
+      <c r="E335" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>335</v>
+      </c>
+      <c r="B336" t="s">
+        <v>44</v>
+      </c>
+      <c r="C336">
+        <v>2</v>
+      </c>
+      <c r="D336" t="s">
+        <v>10</v>
+      </c>
+      <c r="E336" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>336</v>
+      </c>
+      <c r="B337" t="s">
+        <v>44</v>
+      </c>
+      <c r="C337">
+        <v>2</v>
+      </c>
+      <c r="D337" t="s">
+        <v>10</v>
+      </c>
+      <c r="E337" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>337</v>
+      </c>
+      <c r="B338" t="s">
+        <v>44</v>
+      </c>
+      <c r="C338">
+        <v>1</v>
+      </c>
+      <c r="D338" t="s">
+        <v>8</v>
+      </c>
+      <c r="E338" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>338</v>
+      </c>
+      <c r="B339" t="s">
+        <v>44</v>
+      </c>
+      <c r="C339">
+        <v>1</v>
+      </c>
+      <c r="D339" t="s">
+        <v>8</v>
+      </c>
+      <c r="E339" t="s">
+        <v>3</v>
+      </c>
+      <c r="G339" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>339</v>
+      </c>
+      <c r="B340" t="s">
+        <v>44</v>
+      </c>
+      <c r="C340">
+        <v>2</v>
+      </c>
+      <c r="D340" t="s">
+        <v>10</v>
+      </c>
+      <c r="E340" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>340</v>
+      </c>
+      <c r="B341" t="s">
+        <v>44</v>
+      </c>
+      <c r="C341">
+        <v>2</v>
+      </c>
+      <c r="D341" t="s">
+        <v>10</v>
+      </c>
+      <c r="E341" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>341</v>
+      </c>
+      <c r="B342" t="s">
+        <v>48</v>
+      </c>
+      <c r="C342">
+        <v>2</v>
+      </c>
+      <c r="D342" t="s">
+        <v>10</v>
+      </c>
+      <c r="E342" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>342</v>
+      </c>
+      <c r="B343" t="s">
+        <v>49</v>
+      </c>
+      <c r="C343">
+        <v>3</v>
+      </c>
+      <c r="D343" t="s">
+        <v>8</v>
+      </c>
+      <c r="E343" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>343</v>
+      </c>
+      <c r="B344" t="s">
+        <v>50</v>
+      </c>
+      <c r="C344">
+        <v>1</v>
+      </c>
+      <c r="D344" t="s">
+        <v>10</v>
+      </c>
+      <c r="E344" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>344</v>
+      </c>
+      <c r="B345" t="s">
+        <v>49</v>
+      </c>
+      <c r="C345">
+        <v>2</v>
+      </c>
+      <c r="D345" t="s">
+        <v>10</v>
+      </c>
+      <c r="E345" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>345</v>
+      </c>
+      <c r="B346" t="s">
+        <v>49</v>
+      </c>
+      <c r="C346">
+        <v>1</v>
+      </c>
+      <c r="D346" t="s">
+        <v>10</v>
+      </c>
+      <c r="E346" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A347">
+        <v>346</v>
+      </c>
+      <c r="B347" t="s">
+        <v>48</v>
+      </c>
+      <c r="C347">
+        <v>2</v>
+      </c>
+      <c r="D347" t="s">
+        <v>10</v>
+      </c>
+      <c r="E347" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A348">
+        <v>347</v>
+      </c>
+      <c r="B348" t="s">
+        <v>51</v>
+      </c>
+      <c r="C348">
+        <v>2</v>
+      </c>
+      <c r="D348" t="s">
+        <v>10</v>
+      </c>
+      <c r="E348" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A349">
+        <v>348</v>
+      </c>
+      <c r="B349" t="s">
+        <v>52</v>
+      </c>
+      <c r="C349">
+        <v>2</v>
+      </c>
+      <c r="D349" t="s">
+        <v>10</v>
+      </c>
+      <c r="E349" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A350">
+        <v>349</v>
+      </c>
+      <c r="B350" t="s">
+        <v>53</v>
+      </c>
+      <c r="C350">
+        <v>3</v>
+      </c>
+      <c r="D350" t="s">
+        <v>10</v>
+      </c>
+      <c r="E350" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A351">
+        <v>350</v>
+      </c>
+      <c r="B351" t="s">
+        <v>52</v>
+      </c>
+      <c r="C351">
+        <v>2</v>
+      </c>
+      <c r="D351" t="s">
+        <v>10</v>
+      </c>
+      <c r="E351" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A352">
+        <v>351</v>
+      </c>
+      <c r="B352" t="s">
+        <v>54</v>
+      </c>
+      <c r="C352">
+        <v>2</v>
+      </c>
+      <c r="D352" t="s">
+        <v>10</v>
+      </c>
+      <c r="E352" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A353">
+        <v>352</v>
+      </c>
+      <c r="B353" t="s">
+        <v>54</v>
+      </c>
+      <c r="C353">
+        <v>2</v>
+      </c>
+      <c r="D353" t="s">
+        <v>10</v>
+      </c>
+      <c r="E353" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A354">
+        <v>353</v>
+      </c>
+      <c r="B354" t="s">
+        <v>54</v>
+      </c>
+      <c r="C354">
+        <v>1</v>
+      </c>
+      <c r="D354" t="s">
+        <v>10</v>
+      </c>
+      <c r="E354" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A355">
+        <v>354</v>
+      </c>
+      <c r="B355" t="s">
+        <v>54</v>
+      </c>
+      <c r="C355">
+        <v>2</v>
+      </c>
+      <c r="D355" t="s">
+        <v>10</v>
+      </c>
+      <c r="E355" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A356">
+        <v>355</v>
+      </c>
+      <c r="B356" t="s">
+        <v>54</v>
+      </c>
+      <c r="C356">
+        <v>2</v>
+      </c>
+      <c r="D356" t="s">
+        <v>10</v>
+      </c>
+      <c r="E356" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A357">
+        <v>356</v>
+      </c>
+      <c r="B357" t="s">
+        <v>54</v>
+      </c>
+      <c r="C357">
+        <v>1</v>
+      </c>
+      <c r="D357" t="s">
+        <v>8</v>
+      </c>
+      <c r="E357" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A358">
+        <v>357</v>
+      </c>
+      <c r="B358" t="s">
+        <v>54</v>
+      </c>
+      <c r="C358">
+        <v>2</v>
+      </c>
+      <c r="D358" t="s">
+        <v>10</v>
+      </c>
+      <c r="E358" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A359">
+        <v>358</v>
+      </c>
+      <c r="B359" t="s">
+        <v>54</v>
+      </c>
+      <c r="C359">
+        <v>3</v>
+      </c>
+      <c r="D359" t="s">
+        <v>9</v>
+      </c>
+      <c r="E359" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A360">
+        <v>359</v>
+      </c>
+      <c r="B360" t="s">
+        <v>54</v>
+      </c>
+      <c r="C360">
+        <v>2</v>
+      </c>
+      <c r="D360" t="s">
+        <v>9</v>
+      </c>
+      <c r="E360" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A361">
+        <v>360</v>
+      </c>
+      <c r="B361" t="s">
+        <v>54</v>
+      </c>
+      <c r="C361">
+        <v>1</v>
+      </c>
+      <c r="D361" t="s">
+        <v>8</v>
+      </c>
+      <c r="E361" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A362">
+        <v>361</v>
+      </c>
+      <c r="B362" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A363">
+        <v>362</v>
+      </c>
+      <c r="B363" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A364">
+        <v>363</v>
+      </c>
+      <c r="B364" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A365">
+        <v>364</v>
+      </c>
+      <c r="B365" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A366">
+        <v>365</v>
+      </c>
+      <c r="B366" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A367">
+        <v>366</v>
+      </c>
+      <c r="B367" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A368">
+        <v>367</v>
+      </c>
+      <c r="B368" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A369">
+        <v>368</v>
+      </c>
+      <c r="B369" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A370">
+        <v>369</v>
+      </c>
+      <c r="B370" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A371">
+        <v>370</v>
+      </c>
+      <c r="B371" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A372">
+        <v>371</v>
+      </c>
+      <c r="B372" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A373">
+        <v>372</v>
+      </c>
+      <c r="B373" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A374">
+        <v>373</v>
+      </c>
+      <c r="B374" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A375">
+        <v>374</v>
+      </c>
+      <c r="B375" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A376">
+        <v>375</v>
+      </c>
+      <c r="B376" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A377">
+        <v>376</v>
+      </c>
+      <c r="B377" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A378">
+        <v>377</v>
+      </c>
+      <c r="B378" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A379">
+        <v>378</v>
+      </c>
+      <c r="B379" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A380">
+        <v>379</v>
+      </c>
+      <c r="B380" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A381">
+        <v>380</v>
+      </c>
+      <c r="B381" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A382">
+        <v>381</v>
+      </c>
+      <c r="B382" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A383">
+        <v>382</v>
+      </c>
+      <c r="B383" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A384">
+        <v>383</v>
+      </c>
+      <c r="B384" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A385">
+        <v>384</v>
+      </c>
+      <c r="B385" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A386">
+        <v>385</v>
+      </c>
+      <c r="B386" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A387">
+        <v>386</v>
+      </c>
+      <c r="B387" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A388">
+        <v>387</v>
+      </c>
+      <c r="B388" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A389">
+        <v>388</v>
+      </c>
+      <c r="B389" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A390">
+        <v>389</v>
+      </c>
+      <c r="B390" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A391">
+        <v>390</v>
+      </c>
+      <c r="B391" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A392">
+        <v>391</v>
+      </c>
+      <c r="B392" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A393">
+        <v>392</v>
+      </c>
+      <c r="B393" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A394">
+        <v>393</v>
+      </c>
+      <c r="B394" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A395">
+        <v>394</v>
+      </c>
+      <c r="B395" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A396">
+        <v>395</v>
+      </c>
+      <c r="B396" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A397">
+        <v>396</v>
+      </c>
+      <c r="B397" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A398">
+        <v>397</v>
+      </c>
+      <c r="B398" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A399">
+        <v>398</v>
+      </c>
+      <c r="B399" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A400">
+        <v>399</v>
+      </c>
+      <c r="B400" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A401">
+        <v>400</v>
+      </c>
+      <c r="B401" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>